<commit_message>
fiz um monte de coisa
</commit_message>
<xml_diff>
--- a/Aula2.xlsx
+++ b/Aula2.xlsx
@@ -1,35 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AOB" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="planilha2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="teste1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet r:id="rId1" sheetId="1" name="AOB"/>
+    <sheet r:id="rId2" sheetId="2" name="planilha2"/>
+    <sheet r:id="rId3" sheetId="3" name="teste1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>DESCRICAO</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Material de Limpeza</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>1203</t>
+  </si>
+  <si>
+    <t>Material de Consumo</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>1245</t>
+  </si>
+  <si>
+    <t>Materia Prima</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,81 +88,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,124 +394,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>CODIGO</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DESCRICAO</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>VALOR</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Material de Limpeza</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1203</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Material de Consumo</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1700</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1245</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Materia Prima</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>